<commit_message>
Python DataCrawling_(Selenium Version 4 update Program)_22.08.17_(1)
</commit_message>
<xml_diff>
--- a/2.Python/WebCrawler/Excel/data/sidogun.xlsx
+++ b/2.Python/WebCrawler/Excel/data/sidogun.xlsx
@@ -48,688 +48,688 @@
     <t>울릉군</t>
   </si>
   <si>
-    <t>서울특별시 종로구</t>
-  </si>
-  <si>
-    <t>서울특별시 중구</t>
-  </si>
-  <si>
-    <t>서울특별시 용산구</t>
-  </si>
-  <si>
-    <t>서울특별시 성동구</t>
-  </si>
-  <si>
-    <t>서울특별시 광진구</t>
-  </si>
-  <si>
-    <t>서울특별시 동대문구</t>
-  </si>
-  <si>
-    <t>서울특별시 중랑구</t>
-  </si>
-  <si>
-    <t>서울특별시 성북구</t>
-  </si>
-  <si>
-    <t>서울특별시 강북구</t>
-  </si>
-  <si>
-    <t>서울특별시 도봉구</t>
-  </si>
-  <si>
-    <t>서울특별시 노원구</t>
-  </si>
-  <si>
-    <t>서울특별시 은평구</t>
-  </si>
-  <si>
-    <t>서울특별시 서대문구</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구</t>
-  </si>
-  <si>
-    <t>서울특별시 양천구</t>
-  </si>
-  <si>
-    <t>서울특별시 강서구</t>
-  </si>
-  <si>
-    <t>서울특별시 구로구</t>
-  </si>
-  <si>
-    <t>서울특별시 금천구</t>
-  </si>
-  <si>
-    <t>서울특별시 영등포구</t>
-  </si>
-  <si>
-    <t>서울특별시 동작구</t>
-  </si>
-  <si>
-    <t>서울특별시 관악구</t>
-  </si>
-  <si>
-    <t>서울특별시 서초구</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구</t>
-  </si>
-  <si>
-    <t>서울특별시 강동구</t>
-  </si>
-  <si>
-    <t>부산광역시 중구</t>
-  </si>
-  <si>
-    <t>부산광역시 서구</t>
-  </si>
-  <si>
-    <t>부산광역시 동구</t>
-  </si>
-  <si>
-    <t>부산광역시 영도구</t>
-  </si>
-  <si>
-    <t>부산광역시 부산진구</t>
-  </si>
-  <si>
-    <t>부산광역시 동래구</t>
-  </si>
-  <si>
-    <t>부산광역시 남구</t>
-  </si>
-  <si>
-    <t>부산광역시 북구</t>
-  </si>
-  <si>
-    <t>부산광역시 해운대구</t>
-  </si>
-  <si>
-    <t>부산광역시 사하구</t>
-  </si>
-  <si>
-    <t>부산광역시 금정구</t>
-  </si>
-  <si>
-    <t>부산광역시 강서구</t>
-  </si>
-  <si>
-    <t>부산광역시 연제구</t>
-  </si>
-  <si>
-    <t>부산광역시 수영구</t>
-  </si>
-  <si>
-    <t>부산광역시 사상구</t>
-  </si>
-  <si>
-    <t>부산광역시 기장군</t>
-  </si>
-  <si>
-    <t>인천광역시 중구</t>
-  </si>
-  <si>
-    <t>인천광역시 동구</t>
-  </si>
-  <si>
-    <t>인천광역시 미추홀구</t>
-  </si>
-  <si>
-    <t>인천광역시 연수구</t>
-  </si>
-  <si>
-    <t>인천광역시 남동구</t>
-  </si>
-  <si>
-    <t>인천광역시 부평구</t>
-  </si>
-  <si>
-    <t>인천광역시 계양구</t>
-  </si>
-  <si>
-    <t>인천광역시 서구</t>
-  </si>
-  <si>
-    <t>인천광역시 강화군</t>
-  </si>
-  <si>
-    <t>인천광역시 옹진군</t>
-  </si>
-  <si>
-    <t>대구광역시 중구</t>
-  </si>
-  <si>
-    <t>대구광역시 동구</t>
-  </si>
-  <si>
-    <t>대구광역시 서구</t>
-  </si>
-  <si>
-    <t>대구광역시 남구</t>
-  </si>
-  <si>
-    <t>대구광역시 북구</t>
-  </si>
-  <si>
-    <t>대구광역시 수성구</t>
-  </si>
-  <si>
-    <t>대구광역시 달서구</t>
-  </si>
-  <si>
-    <t>대구광역시 달성군</t>
-  </si>
-  <si>
-    <t>대전광역시 동구</t>
-  </si>
-  <si>
-    <t>대전광역시 중구</t>
-  </si>
-  <si>
-    <t>대전광역시 서구</t>
-  </si>
-  <si>
-    <t>대전광역시 유성구</t>
-  </si>
-  <si>
-    <t>대전광역시 대덕구</t>
-  </si>
-  <si>
-    <t>광주광역시 동구</t>
-  </si>
-  <si>
-    <t>광주광역시 서구</t>
-  </si>
-  <si>
-    <t>광주광역시 남구</t>
-  </si>
-  <si>
-    <t>광주광역시 북구</t>
-  </si>
-  <si>
-    <t>광주광역시 광산구</t>
-  </si>
-  <si>
-    <t>울산광역시 중구</t>
-  </si>
-  <si>
-    <t>울산광역시 남구</t>
-  </si>
-  <si>
-    <t>울산광역시 동구</t>
-  </si>
-  <si>
-    <t>울산광역시 북구</t>
-  </si>
-  <si>
-    <t>울산광역시 울주군</t>
-  </si>
-  <si>
-    <t>제주특별자치도 제주시</t>
-  </si>
-  <si>
-    <t>제주특별자치도 서귀포시</t>
-  </si>
-  <si>
-    <t>경기도 수원시</t>
-  </si>
-  <si>
-    <t>경기도 성남시</t>
-  </si>
-  <si>
-    <t>경기도 의정부시</t>
-  </si>
-  <si>
-    <t>경기도 안양시</t>
-  </si>
-  <si>
-    <t>경기도 부천시</t>
-  </si>
-  <si>
-    <t>경기도 광명시</t>
-  </si>
-  <si>
-    <t>경기도 평택시</t>
-  </si>
-  <si>
-    <t>경기도 동두천시</t>
-  </si>
-  <si>
-    <t>경기도 안산시</t>
-  </si>
-  <si>
-    <t>경기도 고양시</t>
-  </si>
-  <si>
-    <t>경기도 과천시</t>
-  </si>
-  <si>
-    <t>경기도 구리시</t>
-  </si>
-  <si>
-    <t>경기도 남양주시</t>
-  </si>
-  <si>
-    <t>경기도 오산시</t>
-  </si>
-  <si>
-    <t>경기도 시흥시</t>
-  </si>
-  <si>
-    <t>경기도 군포시</t>
-  </si>
-  <si>
-    <t>경기도 의왕시</t>
-  </si>
-  <si>
-    <t>경기도 하남시</t>
-  </si>
-  <si>
-    <t>경기도 용인시</t>
-  </si>
-  <si>
-    <t>경기도 파주시</t>
-  </si>
-  <si>
-    <t>경기도 이천시</t>
-  </si>
-  <si>
-    <t>경기도 안성시</t>
-  </si>
-  <si>
-    <t>경기도 김포시</t>
-  </si>
-  <si>
-    <t>경기도 화성시</t>
-  </si>
-  <si>
-    <t>경기도 광주시</t>
-  </si>
-  <si>
-    <t>경기도 양주시</t>
-  </si>
-  <si>
-    <t>경기도 포천시</t>
-  </si>
-  <si>
-    <t>경기도 여주시</t>
-  </si>
-  <si>
-    <t>경기도 연천군</t>
-  </si>
-  <si>
-    <t>경기도 가평군</t>
-  </si>
-  <si>
-    <t>경기도 양평군</t>
-  </si>
-  <si>
-    <t>강원도 춘천시</t>
-  </si>
-  <si>
-    <t>강원도 원주시</t>
-  </si>
-  <si>
-    <t>강원도 강릉시</t>
-  </si>
-  <si>
-    <t>강원도 동해시</t>
-  </si>
-  <si>
-    <t>강원도 태백시</t>
-  </si>
-  <si>
-    <t>강원도 속초시</t>
-  </si>
-  <si>
-    <t>강원도 삼척시</t>
-  </si>
-  <si>
-    <t>강원도 홍천군</t>
-  </si>
-  <si>
-    <t>강원도 횡성군</t>
-  </si>
-  <si>
-    <t>강원도 영월군</t>
-  </si>
-  <si>
-    <t>강원도 평창군</t>
-  </si>
-  <si>
-    <t>강원도 정선군</t>
-  </si>
-  <si>
-    <t>강원도 철원군</t>
-  </si>
-  <si>
-    <t>강원도 화천군</t>
-  </si>
-  <si>
-    <t>강원도 양구군</t>
-  </si>
-  <si>
-    <t>강원도 인제군</t>
-  </si>
-  <si>
-    <t>강원도 고성군</t>
-  </si>
-  <si>
-    <t>강원도 양양군</t>
-  </si>
-  <si>
-    <t>충청북도 청주시</t>
-  </si>
-  <si>
-    <t>충청북도 충주시</t>
-  </si>
-  <si>
-    <t>충청북도 제천시</t>
-  </si>
-  <si>
-    <t>충청북도 보은군</t>
-  </si>
-  <si>
-    <t>충청북도 옥천군</t>
-  </si>
-  <si>
-    <t>충청북도 영동군</t>
-  </si>
-  <si>
-    <t>충청북도 증평군</t>
-  </si>
-  <si>
-    <t>충청북도 진천군</t>
-  </si>
-  <si>
-    <t>충청북도 괴산군</t>
-  </si>
-  <si>
-    <t>충청북도 음성군</t>
-  </si>
-  <si>
-    <t>충청북도 단양군</t>
-  </si>
-  <si>
-    <t>충청남도 천안시</t>
-  </si>
-  <si>
-    <t>충청남도 공주시</t>
-  </si>
-  <si>
-    <t>충청남도 보령시</t>
-  </si>
-  <si>
-    <t>충청남도 아산시</t>
-  </si>
-  <si>
-    <t>충청남도 서산시</t>
-  </si>
-  <si>
-    <t>충청남도 논산시</t>
-  </si>
-  <si>
-    <t>충청남도 계룡시</t>
-  </si>
-  <si>
-    <t>충청남도 당진시</t>
-  </si>
-  <si>
-    <t>충청남도 금산군</t>
-  </si>
-  <si>
-    <t>충청남도 부여군</t>
-  </si>
-  <si>
-    <t>충청남도 서천군</t>
-  </si>
-  <si>
-    <t>충청남도 청양군</t>
-  </si>
-  <si>
-    <t>충청남도 홍성군</t>
-  </si>
-  <si>
-    <t>충청남도 예산군</t>
-  </si>
-  <si>
-    <t>충청남도 태안군</t>
-  </si>
-  <si>
-    <t>전라남도 목포시</t>
-  </si>
-  <si>
-    <t>전라남도 여수시</t>
-  </si>
-  <si>
-    <t>전라남도 순천시</t>
-  </si>
-  <si>
-    <t>전라남도 나주시</t>
-  </si>
-  <si>
-    <t>전라남도 광양시</t>
-  </si>
-  <si>
-    <t>전라남도 담양군</t>
-  </si>
-  <si>
-    <t>전라남도 곡성군</t>
-  </si>
-  <si>
-    <t>전라남도 구례군</t>
-  </si>
-  <si>
-    <t>전라남도 고흥군</t>
-  </si>
-  <si>
-    <t>전라남도 보성군</t>
-  </si>
-  <si>
-    <t>전라남도 화순군</t>
-  </si>
-  <si>
-    <t>전라남도 장흥군</t>
-  </si>
-  <si>
-    <t>전라남도 강진군</t>
-  </si>
-  <si>
-    <t>전라남도 해남군</t>
-  </si>
-  <si>
-    <t>전라남도 영암군</t>
-  </si>
-  <si>
-    <t>전라남도 무안군</t>
-  </si>
-  <si>
-    <t>전라남도 함평군</t>
-  </si>
-  <si>
-    <t>전라남도 영광군</t>
-  </si>
-  <si>
-    <t>전라남도 장성군</t>
-  </si>
-  <si>
-    <t>전라남도 완도군</t>
-  </si>
-  <si>
-    <t>전라남도 진도군</t>
-  </si>
-  <si>
-    <t>전라남도 신안군</t>
-  </si>
-  <si>
-    <t>전라북도 전주시</t>
-  </si>
-  <si>
-    <t>전라북도 군산시</t>
-  </si>
-  <si>
-    <t>전라북도 익산시</t>
-  </si>
-  <si>
-    <t>전라북도 정읍시</t>
-  </si>
-  <si>
-    <t>전라북도 남원시</t>
-  </si>
-  <si>
-    <t>전라북도 김제시</t>
-  </si>
-  <si>
-    <t>전라북도 완주군</t>
-  </si>
-  <si>
-    <t>전라북도 진안군</t>
-  </si>
-  <si>
-    <t>전라북도 무주군</t>
-  </si>
-  <si>
-    <t>전라북도 장수군</t>
-  </si>
-  <si>
-    <t>전라북도 임실군</t>
-  </si>
-  <si>
-    <t>전라북도 순창군</t>
-  </si>
-  <si>
-    <t>전라북도 고창군</t>
-  </si>
-  <si>
-    <t>전라북도 부안군</t>
-  </si>
-  <si>
-    <t>경상남도 창원시</t>
-  </si>
-  <si>
-    <t>경상남도 진주시</t>
-  </si>
-  <si>
-    <t>경상남도 통영시</t>
-  </si>
-  <si>
-    <t>경상남도 사천시</t>
-  </si>
-  <si>
-    <t>경상남도 김해시</t>
-  </si>
-  <si>
-    <t>경상남도 밀양시</t>
-  </si>
-  <si>
-    <t>경상남도 거제시</t>
-  </si>
-  <si>
-    <t>경상남도 양산시</t>
-  </si>
-  <si>
-    <t>경상남도 의령군</t>
-  </si>
-  <si>
-    <t>경상남도 함안군</t>
-  </si>
-  <si>
-    <t>경상남도 창녕군</t>
-  </si>
-  <si>
-    <t>경상남도 고성군</t>
-  </si>
-  <si>
-    <t>경상남도 남해군</t>
-  </si>
-  <si>
-    <t>경상남도 하동군</t>
-  </si>
-  <si>
-    <t>경상남도 산청군</t>
-  </si>
-  <si>
-    <t>경상남도 함양군</t>
-  </si>
-  <si>
-    <t>경상남도 거창군</t>
-  </si>
-  <si>
-    <t>경상남도 합천군</t>
-  </si>
-  <si>
-    <t>경상북도 포항시</t>
-  </si>
-  <si>
-    <t>경상북도 경주시</t>
-  </si>
-  <si>
-    <t>경상북도 김천시</t>
-  </si>
-  <si>
-    <t>경상북도 안동시</t>
-  </si>
-  <si>
-    <t>경상북도 구미시</t>
-  </si>
-  <si>
-    <t>경상북도 영주시</t>
-  </si>
-  <si>
-    <t>경상북도 영천시</t>
-  </si>
-  <si>
-    <t>경상북도 상주시</t>
-  </si>
-  <si>
-    <t>경상북도 문경시</t>
-  </si>
-  <si>
-    <t>경상북도 경산시</t>
-  </si>
-  <si>
-    <t>경상북도 군위군</t>
-  </si>
-  <si>
-    <t>경상북도 의성군</t>
-  </si>
-  <si>
-    <t>경상북도 청송군</t>
-  </si>
-  <si>
-    <t>경상북도 영양군</t>
-  </si>
-  <si>
-    <t>경상북도 영덕군</t>
-  </si>
-  <si>
-    <t>경상북도 청도군</t>
-  </si>
-  <si>
-    <t>경상북도 고령군</t>
-  </si>
-  <si>
-    <t>경상북도 성주군</t>
-  </si>
-  <si>
-    <t>경상북도 칠곡군</t>
-  </si>
-  <si>
-    <t>경상북도 예천군</t>
-  </si>
-  <si>
-    <t>경상북도 봉화군</t>
-  </si>
-  <si>
-    <t>경상북도 울진군</t>
-  </si>
-  <si>
-    <t>경상북도 울릉군</t>
+    <t xml:space="preserve"> 서울특별시 종로구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 중구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 용산구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 성동구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 광진구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 동대문구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 중랑구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 성북구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 강북구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 도봉구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 노원구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 은평구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 서대문구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 마포구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 양천구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 강서구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 구로구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 금천구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 영등포구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 동작구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 관악구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 서초구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 강남구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 송파구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 서울특별시 강동구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 중구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 서구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 동구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 영도구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 부산진구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 동래구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 남구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 북구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 해운대구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 사하구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 금정구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 강서구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 연제구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 수영구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 사상구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 부산광역시 기장군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 인천광역시 중구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 인천광역시 동구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 인천광역시 미추홀구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 인천광역시 연수구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 인천광역시 남동구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 인천광역시 부평구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 인천광역시 계양구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 인천광역시 서구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 인천광역시 강화군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 인천광역시 옹진군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 대구광역시 중구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 대구광역시 동구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 대구광역시 서구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 대구광역시 남구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 대구광역시 북구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 대구광역시 수성구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 대구광역시 달서구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 대구광역시 달성군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 대전광역시 동구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 대전광역시 중구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 대전광역시 서구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 대전광역시 유성구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 대전광역시 대덕구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 광주광역시 동구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 광주광역시 서구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 광주광역시 남구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 광주광역시 북구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 광주광역시 광산구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 울산광역시 중구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 울산광역시 남구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 울산광역시 동구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 울산광역시 북구</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 울산광역시 울주군</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  제주특별자치도 제주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 제주특별자치도 서귀포시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 수원시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 성남시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 의정부시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 안양시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 부천시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 광명시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 평택시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 동두천시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 안산시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 고양시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 과천시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 구리시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 남양주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 오산시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 시흥시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 군포시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 의왕시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 하남시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 용인시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 파주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 이천시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 안성시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 김포시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 화성시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 광주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 양주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 포천시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 여주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 연천군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 가평군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경기도 양평군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 춘천시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 원주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 강릉시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 동해시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 태백시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 속초시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 삼척시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 홍천군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 횡성군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 영월군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 평창군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 정선군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 철원군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 화천군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 양구군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 인제군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 고성군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 강원도 양양군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청북도 청주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청북도 충주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청북도 제천시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청북도 보은군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청북도 옥천군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청북도 영동군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청북도 증평군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청북도 진천군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청북도 괴산군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청북도 음성군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청북도 단양군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청남도 천안시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청남도 공주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청남도 보령시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청남도 아산시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청남도 서산시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청남도 논산시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청남도 계룡시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청남도 당진시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청남도 금산군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청남도 부여군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청남도 서천군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청남도 청양군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청남도 홍성군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청남도 예산군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 충청남도 태안군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 목포시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 여수시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 순천시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 나주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 광양시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 담양군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 곡성군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 구례군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 고흥군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 보성군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 화순군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 장흥군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 강진군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 해남군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 영암군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 무안군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 함평군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 영광군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 장성군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 완도군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 진도군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라남도 신안군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라북도 전주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라북도 군산시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라북도 익산시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라북도 정읍시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라북도 남원시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라북도 김제시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라북도 완주군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라북도 진안군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라북도 무주군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라북도 장수군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라북도 임실군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라북도 순창군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라북도 고창군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 전라북도 부안군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 창원시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 진주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 통영시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 사천시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 김해시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 밀양시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 거제시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 양산시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 의령군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 함안군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 창녕군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 고성군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 남해군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 하동군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 산청군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 함양군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 거창군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상남도 합천군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 포항시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 경주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 김천시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 안동시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 구미시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 영주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 영천시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 상주시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 문경시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 경산시</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 군위군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 의성군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 청송군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 영양군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 영덕군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 청도군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 고령군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 성주군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 칠곡군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 예천군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 봉화군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 울진군</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 경상북도 울릉군</t>
   </si>
 </sst>
 </file>
@@ -1082,20 +1082,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="G223" sqref="G223"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="A227" sqref="A227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="7.125" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="8" max="8" width="7.125" customWidth="1"/>
-    <col min="9" max="10" width="9" customWidth="1"/>
-    <col min="11" max="13" width="7.125" customWidth="1"/>
-    <col min="15" max="17" width="7.125" customWidth="1"/>
+    <col min="2" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="7" max="7" width="7.125" customWidth="1"/>
+    <col min="8" max="9" width="9" customWidth="1"/>
+    <col min="10" max="12" width="7.125" customWidth="1"/>
+    <col min="14" max="16" width="7.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>